<commit_message>
:package: caderno de anotações melhorado com alguns botões funcionais
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,277 +424,284 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>data</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>questao_id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>disciplina</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>assunto</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>anotacao</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>26/12/2025 05:10</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>276</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Português</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Ambiguidade</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Tenho que rever essa questão, tinha certeza que a opção A não tinha ambiguidade por "funcionários" está no plural e o pronome "seu" no singular</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>26/12/2025 05:15</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>435</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Logística</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Rever as características dos modais de trasporte</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>26/12/2025 05:22</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>503</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Engenharia Organizacional</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Investigar essa questão mais afundo. parece ser de planejamento estratégico, mas para mim, ficou muito aberta</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>26/12/2025 05:25</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>442</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Logística</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Investigar o que é cabotagem</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>26/12/2025 05:55</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>471</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Processos Decisórios</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Mudar o assunto dessa disciplina para Processos Decisórios. Estudar mais esse assunto</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>26/12/2025 06:11</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>436</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Logística</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Errando mais uma questão por confundir incorreta com correta</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>26/12/2025 06:21</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>554</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Engenharia de Métodos e Processos</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Investigar como é que aumento da eficiencia pode aumentar o tempo gasto ao inves de diminuir</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>26/12/2025 07:00</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>633</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Engenharia de Produto</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Corrigir o layout dessa questão</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>26/12/2025 07:03</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>393</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Conhecimentos Específicos</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Gestão da Produção e Operações</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Rever essa explicação nos comentários</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>26/12/2025 08:00</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>614</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Conhecimentos Específicos</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Gestão da Qualidade</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Analisar essa questã, pois a III para mim tb parece verdadeira</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
:up: ultimo commit antes de tentar adicionar data de inserção no db das questoes
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,62 +649,6 @@
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>26/12/2025 07:00</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>633</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Conhecimentos Específicos</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Engenharia de Produto</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Corrigir o layout dessa questão</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>26/12/2025 07:03</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>393</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Conhecimentos Específicos</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Gestão da Produção e Operações</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Rever essa explicação nos comentários</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:checkered_flag: praticar e simulado unificados
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,6 +649,62 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>27/12/2025 00:51</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>542</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Estudar TPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>27/12/2025 00:52</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>542</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Estudar esse tal de 8 S</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:checkered_flag: logica de randomização por respostas e datas implementadas, indo para um melhoramento
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -705,6 +705,298 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>27/12/2025 05:40</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>937</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Pronouns</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Retirar os números de linhas no meio do testo</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>27/12/2025 05:43</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>935</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Salvar a palavra yield no sistema de english learning. nesse caso foi um verbo que teve o mesmo significado de produce</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>27/12/2025 05:46</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>934</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Incluir palavra Hence no english learnig</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>27/12/2025 05:48</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>933</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Analisar esse erro, marquei letra C</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>27/12/2025 06:28</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>263</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sinônimo E Antônimo</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Criar um flashcard do significado da palavra resignação</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>27/12/2025 06:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Correlação Verbal</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Estudar esssa tal uma variação "estranha/formal" "Chovesse" com o mesmo sentido de "choveria"</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>27/12/2025 06:38</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Investigar o valor semântico de concessão e conformidade, marquei conformidade, letra D, nessa questão</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>27/12/2025 08:40</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>279</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Coesão</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>colocar em negrito a palavra "que" nessa questão</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>27/12/2025 08:41</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>262</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Sinônimo E Antônimo</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>repetida?</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>27/12/2025 08:43</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>261</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Sinônimo E Antônimo</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Criar um flashcard de significado da palavra Reminiscência</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: ultimo commit antes de tentar implementar um gerenciado de textos no banco
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,15 +567,15 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26/12/2025 05:55</t>
+          <t>26/12/2025 06:11</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>471</v>
+        <v>436</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -584,26 +584,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Processos Decisórios</t>
+          <t>Logística</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Mudar o assunto dessa disciplina para Processos Decisórios. Estudar mais esse assunto</t>
+          <t>Errando mais uma questão por confundir incorreta com correta</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26/12/2025 06:11</t>
+          <t>26/12/2025 06:21</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>436</v>
+        <v>554</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -612,26 +612,26 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Logística</t>
+          <t>Engenharia de Métodos e Processos</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Errando mais uma questão por confundir incorreta com correta</t>
+          <t>Investigar como é que aumento da eficiencia pode aumentar o tempo gasto ao inves de diminuir</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>26/12/2025 06:21</t>
+          <t>27/12/2025 00:51</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Engenharia de Métodos e Processos</t>
+          <t>Gestão da Manutenção e Confiabilidade</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Investigar como é que aumento da eficiencia pode aumentar o tempo gasto ao inves de diminuir</t>
+          <t>Estudar TPM</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27/12/2025 00:51</t>
+          <t>27/12/2025 00:52</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -673,327 +673,93 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Estudar TPM</t>
+          <t>Estudar esse tal de 8 S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>27/12/2025 00:52</t>
+          <t>27/12/2025 05:40</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>542</v>
+        <v>937</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Conhecimentos Específicos</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Gestão da Manutenção e Confiabilidade</t>
+          <t>Pronouns</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Estudar esse tal de 8 S</t>
+          <t>Retirar os números de linhas no meio do testo</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27/12/2025 05:40</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>937</v>
+          <t>27/12/2025 06:38</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Pronouns</t>
+          <t>Conjunção</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Retirar os números de linhas no meio do testo</t>
+          <t>Investigar o valor semântico de concessão e conformidade, marquei conformidade, letra D, nessa questão</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>27/12/2025 05:43</t>
+          <t>27/12/2025 10:14</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>935</v>
+        <v>121</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Semantic</t>
+          <t>Verbos Traiçoeiros</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Salvar a palavra yield no sistema de english learning. nesse caso foi um verbo que teve o mesmo significado de produce</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>27/12/2025 05:46</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>934</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Semantic</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Incluir palavra Hence no english learnig</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>27/12/2025 05:48</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>933</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Interpretação de Texto</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Analisar esse erro, marquei letra C</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>27/12/2025 06:28</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>263</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Sinônimo E Antônimo</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Criar um flashcard do significado da palavra resignação</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>27/12/2025 06:35</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>125</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Correlação Verbal</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Estudar esssa tal uma variação "estranha/formal" "Chovesse" com o mesmo sentido de "choveria"</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>27/12/2025 06:38</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Conjunção</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Investigar o valor semântico de concessão e conformidade, marquei conformidade, letra D, nessa questão</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>27/12/2025 08:40</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>279</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Coesão</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>colocar em negrito a palavra "que" nessa questão</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>27/12/2025 08:41</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>262</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Sinônimo E Antônimo</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>repetida?</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>27/12/2025 08:43</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>261</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Português</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Sinônimo E Antônimo</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Criar um flashcard de significado da palavra Reminiscência</t>
+          <t>Estudar mais esse assunto</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
:up: algumas questões respondidas, iniciando tentativa de correção do leitor de pdf nao estar captando as questoes comentadas da disciplina de Cont Ger
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -763,6 +763,148 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>22</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>29/12/2025 04:28</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>545</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Gestão da Manutenção e Confiabilidade</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Criar um formulários/flashcards para as fórmulas desse assunto</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>23</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>29/12/2025 04:45</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Estatística</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Medidas de Variabilidade</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Revisar medidas de variabilidade em tabelas de frequencias</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>24</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>29/12/2025 04:46</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1191</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Estatística</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Testes de Hipóteses</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>p-value, faço nem ideia de como se calcula</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>25</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>29/12/2025 04:49</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1241</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Estatística</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ANOVA</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Faço nem ideia</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>26</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>29/12/2025 04:58</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>954</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Pronouns</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Organizar esse texto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: alguns assuntos removidos por julgar nao necessários
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,120 +791,6 @@
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>23</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>29/12/2025 04:45</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1007</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Estatística</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Medidas de Variabilidade</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Revisar medidas de variabilidade em tabelas de frequencias</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>24</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>29/12/2025 04:46</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1191</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Estatística</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Testes de Hipóteses</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>p-value, faço nem ideia de como se calcula</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>25</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>29/12/2025 04:49</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1241</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Estatística</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ANOVA</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Faço nem ideia</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>26</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>29/12/2025 04:58</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>954</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Pronouns</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Organizar esse texto</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:package: plano de estudos melhorado
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,34 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>23</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>31/12/2025 02:46</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>515</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Layout e Arranjos Físicos</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Rever tipos de layout</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: algumas questões respondidas
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -765,15 +765,15 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>29/12/2025 04:28</t>
+          <t>31/12/2025 02:46</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>545</v>
+        <v>515</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -782,26 +782,26 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Gestão da Manutenção e Confiabilidade</t>
+          <t>Layout e Arranjos Físicos</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Criar um formulários/flashcards para as fórmulas desse assunto</t>
+          <t>Rever tipos de layout</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>31/12/2025 02:46</t>
+          <t>31/12/2025 02:53</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -815,7 +815,372 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Rever tipos de layout</t>
+          <t>não me atentei a palavar VARIEDADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>25</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>31/12/2025 06:12</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>756</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Gestão da Cadeia de Suprimentos</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>retirar os parenteses dos finais das alternativas</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>26</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>31/12/2025 11:03</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1421</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Contabilidade Gerencial</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Contabilidade Básica</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Corrigir o gabarito dessa questão</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>27</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>31/12/2025 11:31</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>123</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Verbos Traiçoeiros</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>arrumar essa questão, tirar os gabaritos da alternativa E</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>28</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>31/12/2025 11:50</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>275</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Ambiguidade</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Tirar duvidas sobre essa questão se possível, a se sentar não seria o equivalente a sentando? se sim essa frase também é ambígua</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>29</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>31/12/2025 11:55</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>225</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Regência Verbal</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>O verbo “querer”, no sentido de “estimar”/“querer bem a”, é VTI e exige a preposição “a”</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>30</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:11</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>222</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Regência Verbal</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>só errei essa questão porque tem dois QUEs nas alternativa E, e como nenhum veio destacado, considerei o primeiro, mas era preciso considerar o segundo para acertar a questão.
+Corrigir essa questão: marcar todos os QUEs, na E, destacar apenas o segundo</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>31</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:12</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>222</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Regência Verbal</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Como assim verbo VTI exige preposição?</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:25</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>180</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Travessão</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>editar essa questão, a alternativa é foi cortada porque disparou um corte no algoritimo de leitura por causa da palavra "comentário"</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>33</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:30</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>308</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Coesão</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Corrigir esse texto, quebras de linhas</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>34</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:32</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>294</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Coesão</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Arrumar esse tal destaque. Deve ser no pronome "lo"</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>35</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:35</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>288</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Coesão</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>extrair o texto dessa imagem e vinculá-lo a essa questão</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>36</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:42</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>281</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Coesão</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Tentar identificar essas tais palavras em destaque, acertei essa questão prativamente dando um tiro no escuro</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>37</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>31/12/2025 12:45</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>303</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Reescritura</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Extrair o texto dessa imagem e vinculá-lo à questão</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
:up: algumas questoes respondidas, ultimo commit antes de implementar leitura de pdf de provas
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -455,15 +455,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26/12/2025 05:15</t>
+          <t>26/12/2025 05:25</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -477,51 +477,51 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Rever as características dos modais de trasporte</t>
+          <t>Investigar o que é cabotagem</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26/12/2025 05:25</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>442</v>
+          <t>27/12/2025 06:38</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Conhecimentos Específicos</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Logística</t>
+          <t>Conjunção</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Investigar o que é cabotagem</t>
+          <t>Investigar o valor semântico de concessão e conformidade, marquei conformidade, letra D, nessa questão</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27/12/2025 06:38</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+          <t>27/12/2025 10:14</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>121</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -530,82 +530,82 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Conjunção</t>
+          <t>Verbos Traiçoeiros</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Investigar o valor semântico de concessão e conformidade, marquei conformidade, letra D, nessa questão</t>
+          <t>Estudar mais esse assunto</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>27/12/2025 10:14</t>
+          <t>31/12/2025 02:53</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>121</v>
+        <v>507</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Conhecimentos Específicos</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Verbos Traiçoeiros</t>
+          <t>Layout e Arranjos Físicos</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Estudar mais esse assunto</t>
+          <t>não me atentei a palavar VARIEDADE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31/12/2025 02:53</t>
+          <t>31/12/2025 11:50</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>507</v>
+        <v>275</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Conhecimentos Específicos</t>
+          <t>Português</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Layout e Arranjos Físicos</t>
+          <t>Ambiguidade</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>não me atentei a palavar VARIEDADE</t>
+          <t>Tirar duvidas sobre essa questão se possível, a se sentar não seria o equivalente a sentando? se sim essa frase também é ambígua</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>31/12/2025 11:50</t>
+          <t>31/12/2025 11:55</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -614,26 +614,26 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ambiguidade</t>
+          <t>Regência Verbal</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Tirar duvidas sobre essa questão se possível, a se sentar não seria o equivalente a sentando? se sim essa frase também é ambígua</t>
+          <t>O verbo “querer”, no sentido de “estimar”/“querer bem a”, é VTI e exige a preposição “a”</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31/12/2025 11:55</t>
+          <t>31/12/2025 12:12</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -647,63 +647,63 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>O verbo “querer”, no sentido de “estimar”/“querer bem a”, é VTI e exige a preposição “a”</t>
+          <t>Como assim verbo VTI exige preposição?</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>31/12/2025 12:12</t>
+          <t>09/01/2026 10:57</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>222</v>
+        <v>1810</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Português</t>
+          <t>Conhecimentos Específicos</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Regência Verbal</t>
+          <t>Logística</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Como assim verbo VTI exige preposição?</t>
+          <t>Criar flashcards para o conteúdo de logística da transpetro</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>01/01/2026 04:21</t>
+          <t>09/01/2026 11:07</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1284</v>
+        <v>1811</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Matemática Financeira</t>
+          <t>Conhecimentos Específicos</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Juros Compostos</t>
+          <t>Logística</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Criar um flashcard com as propriedades dos logarítimos</t>
+          <t>Retirar ruídos dessa questão</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
:up: algumas questoes respondidas, o sistema conseguiu ler as questoes do pdf de prova
</commit_message>
<xml_diff>
--- a/banco_de_dados/caderno_anotacoes.xlsx
+++ b/banco_de_dados/caderno_anotacoes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,34 +679,6 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>33</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>09/01/2026 11:07</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1811</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Conhecimentos Específicos</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Logística</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Retirar ruídos dessa questão</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>